<commit_message>
Add household surplus computations
</commit_message>
<xml_diff>
--- a/model/Outputs/0. Initial Solution/Output_0_40.xlsx
+++ b/model/Outputs/0. Initial Solution/Output_0_40.xlsx
@@ -440,7 +440,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -501,6 +501,46 @@
       </c>
       <c r="B6" t="n">
         <v>4063037.097587747</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Wasted Prosumer Surplus</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>342857.5917216506</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Total Wasted Prosumer Surplus</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>342857.5917216506</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Unmet Demand</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>25277.78700766068</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Total Unmet Demand</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>25277.78700766068</v>
       </c>
     </row>
   </sheetData>
@@ -26154,7 +26194,7 @@
         <v>1020614.467526005</v>
       </c>
       <c r="P2" t="n">
-        <v>968714.0067689738</v>
+        <v>968714.0067689735</v>
       </c>
     </row>
     <row r="3">
@@ -26329,7 +26369,7 @@
         <v>555657.8366644464</v>
       </c>
       <c r="E6" t="n">
-        <v>243611.0804004286</v>
+        <v>243611.0804004285</v>
       </c>
       <c r="F6" t="n">
         <v>547995.79512663</v>
@@ -26341,7 +26381,7 @@
         <v>564424.5670149443</v>
       </c>
       <c r="I6" t="n">
-        <v>566258.3915408098</v>
+        <v>566258.3915408097</v>
       </c>
       <c r="J6" t="n">
         <v>268612.6705113701</v>
@@ -26350,19 +26390,19 @@
         <v>533250.9719164991</v>
       </c>
       <c r="L6" t="n">
-        <v>548672.0700031896</v>
+        <v>548672.0700031894</v>
       </c>
       <c r="M6" t="n">
         <v>576946.4244184083</v>
       </c>
       <c r="N6" t="n">
-        <v>578823.4738435991</v>
+        <v>578823.4738435993</v>
       </c>
       <c r="O6" t="n">
         <v>321856.749251524</v>
       </c>
       <c r="P6" t="n">
-        <v>551843.8601907562</v>
+        <v>551843.8601907559</v>
       </c>
     </row>
   </sheetData>

</xml_diff>